<commit_message>
reflects new db fields and table
</commit_message>
<xml_diff>
--- a/CookingApp/DataBase/schema.xlsx
+++ b/CookingApp/DataBase/schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ailish\Documents\OSU\361\project\cooking-curriculum\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ailish\Documents\OSU\361\project\cooking-curriculum\cooking-curriculum\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCEC2D1-9834-4FB3-BE6C-0F54156F1E0F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C8996D-675C-4E85-AD3D-A33AFDA4BF1C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" xr2:uid="{72953FF3-AD13-4F17-80A9-A60DD70B2A76}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="56">
   <si>
     <t>Table Name</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>dateStatus</t>
+  </si>
+  <si>
+    <t>recipeIngredients</t>
+  </si>
+  <si>
+    <t>ingredientID</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>img_url</t>
+  </si>
+  <si>
+    <t>stepOrder</t>
   </si>
 </sst>
 </file>
@@ -585,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86304BA0-CAC6-4B37-B172-DD84F9F9BB9C}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -746,7 +764,7 @@
     <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>29</v>
@@ -756,40 +774,38 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>35</v>
@@ -798,12 +814,14 @@
     <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
@@ -811,50 +829,48 @@
     <row r="17" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>35</v>
@@ -863,7 +879,7 @@
     <row r="21" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>28</v>
@@ -878,50 +894,50 @@
     <row r="22" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>35</v>
@@ -930,7 +946,7 @@
     <row r="26" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>28</v>
@@ -945,49 +961,51 @@
     <row r="27" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E30" s="2" t="s">
         <v>35</v>
       </c>
@@ -995,50 +1013,48 @@
     <row r="31" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>35</v>
@@ -1047,12 +1063,14 @@
     <row r="35" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1060,50 +1078,48 @@
     <row r="36" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>35</v>
@@ -1112,12 +1128,14 @@
     <row r="40" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>35</v>
       </c>
@@ -1125,36 +1143,38 @@
     <row r="41" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+    <row r="42" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="43" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
         <v>35</v>
       </c>
@@ -1162,79 +1182,77 @@
     <row r="44" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>35</v>
-      </c>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
@@ -1244,79 +1262,75 @@
     <row r="50" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+    <row r="51" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="52" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E55" s="2" t="s">
         <v>35</v>
       </c>
@@ -1324,28 +1338,150 @@
     <row r="56" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2" t="s">
+      <c r="D59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A51:E51"/>
+  <mergeCells count="11">
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added timeToCookMins col to recipe table
</commit_message>
<xml_diff>
--- a/CookingApp/DataBase/schema.xlsx
+++ b/CookingApp/DataBase/schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ailish\Documents\OSU\361\project\cooking-curriculum\cooking-curriculum\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ailish\Documents\OSU\361\project\cooking-curriculum\CookingApp\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C8996D-675C-4E85-AD3D-A33AFDA4BF1C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44695223-F0CD-4706-A890-DCCE954149AB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" xr2:uid="{72953FF3-AD13-4F17-80A9-A60DD70B2A76}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="57">
   <si>
     <t>Table Name</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>stepOrder</t>
+  </si>
+  <si>
+    <t>timeToCookMins</t>
   </si>
 </sst>
 </file>
@@ -603,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86304BA0-CAC6-4B37-B172-DD84F9F9BB9C}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -764,10 +767,10 @@
     <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
@@ -777,7 +780,7 @@
     <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>29</v>
@@ -787,40 +790,38 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>35</v>
@@ -829,12 +830,14 @@
     <row r="17" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>35</v>
       </c>
@@ -842,50 +845,48 @@
     <row r="18" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>35</v>
@@ -894,7 +895,7 @@
     <row r="22" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -909,50 +910,50 @@
     <row r="23" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="C24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>35</v>
@@ -961,7 +962,7 @@
     <row r="27" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>28</v>
@@ -976,49 +977,51 @@
     <row r="28" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1026,50 +1029,48 @@
     <row r="32" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>35</v>
@@ -1078,12 +1079,14 @@
     <row r="36" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1091,50 +1094,48 @@
     <row r="37" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>35</v>
@@ -1143,12 +1144,14 @@
     <row r="41" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>35</v>
       </c>
@@ -1156,7 +1159,7 @@
     <row r="42" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>29</v>
@@ -1169,10 +1172,10 @@
     <row r="43" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
@@ -1182,50 +1185,48 @@
     <row r="44" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>35</v>
@@ -1234,7 +1235,7 @@
     <row r="48" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>28</v>
@@ -1249,23 +1250,25 @@
     <row r="49" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
@@ -1275,7 +1278,7 @@
     <row r="51" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>28</v>
@@ -1288,7 +1291,7 @@
     <row r="52" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>28</v>
@@ -1301,50 +1304,48 @@
     <row r="53" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>35</v>
@@ -1353,7 +1354,7 @@
     <row r="57" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>28</v>
@@ -1368,12 +1369,14 @@
     <row r="58" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>35</v>
       </c>
@@ -1381,50 +1384,48 @@
     <row r="59" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>35</v>
@@ -1433,12 +1434,14 @@
     <row r="63" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>35</v>
       </c>
@@ -1446,7 +1449,7 @@
     <row r="64" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>31</v>
@@ -1459,29 +1462,42 @@
     <row r="65" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="66" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A39:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>